<commit_message>
Added 1 More Meja
Added Meja 13
</commit_message>
<xml_diff>
--- a/Objek/denah palgading.xlsx
+++ b/Objek/denah palgading.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7905" tabRatio="272"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7908" tabRatio="272"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Kasir</t>
   </si>
@@ -99,13 +99,16 @@
   </si>
   <si>
     <t>9420 - 9390</t>
+  </si>
+  <si>
+    <t>9526 - 9471</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,6 +139,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -399,7 +409,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -416,6 +426,114 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="180" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -425,113 +543,26 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="180"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -820,136 +851,136 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:Y34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7:T9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
     <col min="5" max="5" width="6" customWidth="1"/>
-    <col min="6" max="6" width="4.42578125" customWidth="1"/>
-    <col min="7" max="7" width="2.85546875" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="2.5703125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="3.85546875" customWidth="1"/>
-    <col min="10" max="10" width="3.7109375" customWidth="1"/>
-    <col min="11" max="11" width="2.85546875" customWidth="1"/>
-    <col min="17" max="18" width="9.140625" customWidth="1"/>
-    <col min="20" max="20" width="9.42578125" customWidth="1"/>
-    <col min="21" max="21" width="11.42578125" customWidth="1"/>
-    <col min="22" max="22" width="3.5703125" customWidth="1"/>
+    <col min="6" max="6" width="4.44140625" customWidth="1"/>
+    <col min="7" max="7" width="2.88671875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="2.5546875" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="3.88671875" customWidth="1"/>
+    <col min="10" max="10" width="3.6640625" customWidth="1"/>
+    <col min="11" max="11" width="2.88671875" customWidth="1"/>
+    <col min="17" max="18" width="9.109375" customWidth="1"/>
+    <col min="20" max="20" width="9.44140625" customWidth="1"/>
+    <col min="21" max="21" width="11.44140625" customWidth="1"/>
+    <col min="22" max="22" width="3.5546875" customWidth="1"/>
     <col min="23" max="23" width="3" customWidth="1"/>
-    <col min="24" max="24" width="3.42578125" customWidth="1"/>
-    <col min="25" max="25" width="3.5703125" customWidth="1"/>
-    <col min="26" max="26" width="9.42578125" customWidth="1"/>
+    <col min="24" max="24" width="3.44140625" customWidth="1"/>
+    <col min="25" max="25" width="3.5546875" customWidth="1"/>
+    <col min="26" max="26" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K5" s="41" t="s">
+    <row r="4" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="2:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="32" t="s">
+      <c r="L5" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
-      <c r="S5" s="33"/>
-      <c r="T5" s="33"/>
-      <c r="U5" s="34"/>
-      <c r="V5" s="41" t="s">
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
+      <c r="S5" s="34"/>
+      <c r="T5" s="34"/>
+      <c r="U5" s="35"/>
+      <c r="V5" s="15" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="41"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
-      <c r="P6" s="36"/>
-      <c r="Q6" s="36"/>
-      <c r="R6" s="36"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="36"/>
-      <c r="U6" s="37"/>
-      <c r="V6" s="41"/>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="K6" s="15"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="37"/>
+      <c r="N6" s="37"/>
+      <c r="O6" s="37"/>
+      <c r="P6" s="37"/>
+      <c r="Q6" s="37"/>
+      <c r="R6" s="37"/>
+      <c r="S6" s="37"/>
+      <c r="T6" s="37"/>
+      <c r="U6" s="38"/>
+      <c r="V6" s="15"/>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C7" s="19"/>
-      <c r="K7" s="41"/>
+      <c r="K7" s="15"/>
       <c r="M7" s="24">
         <v>1</v>
       </c>
-      <c r="N7" s="38"/>
-      <c r="O7" s="38"/>
-      <c r="P7" s="38"/>
-      <c r="Q7" s="38"/>
-      <c r="R7" s="38"/>
-      <c r="S7" s="38"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="39"/>
+      <c r="P7" s="39"/>
+      <c r="Q7" s="39"/>
+      <c r="R7" s="39"/>
+      <c r="S7" s="39"/>
       <c r="T7" s="25"/>
-      <c r="V7" s="41"/>
-    </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V7" s="15"/>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C8" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="41"/>
+      <c r="K8" s="15"/>
       <c r="M8" s="24"/>
-      <c r="N8" s="38"/>
-      <c r="O8" s="38"/>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="38"/>
-      <c r="R8" s="38"/>
-      <c r="S8" s="38"/>
+      <c r="N8" s="39"/>
+      <c r="O8" s="39"/>
+      <c r="P8" s="39"/>
+      <c r="Q8" s="39"/>
+      <c r="R8" s="39"/>
+      <c r="S8" s="39"/>
       <c r="T8" s="25"/>
-      <c r="V8" s="41"/>
-    </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="V8" s="15"/>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
       <c r="C9" s="21"/>
-      <c r="J9" s="40" t="s">
+      <c r="J9" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="41"/>
+      <c r="K9" s="15"/>
       <c r="M9" s="26"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="39"/>
-      <c r="Q9" s="39"/>
-      <c r="R9" s="39"/>
-      <c r="S9" s="39"/>
+      <c r="N9" s="40"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="40"/>
+      <c r="Q9" s="40"/>
+      <c r="R9" s="40"/>
+      <c r="S9" s="40"/>
       <c r="T9" s="27"/>
-      <c r="V9" s="41"/>
-      <c r="W9" s="40" t="s">
+      <c r="V9" s="15"/>
+      <c r="W9" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C10" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="40"/>
-      <c r="K10" s="41"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="15"/>
       <c r="L10" t="s">
         <v>16</v>
       </c>
       <c r="U10" t="s">
         <v>16</v>
       </c>
-      <c r="V10" s="41"/>
-      <c r="W10" s="40"/>
-    </row>
-    <row r="11" spans="2:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V10" s="15"/>
+      <c r="W10" s="14"/>
+    </row>
+    <row r="11" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C11" s="19"/>
-      <c r="J11" s="40"/>
+      <c r="J11" s="14"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -961,28 +992,28 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="3"/>
-      <c r="W11" s="40"/>
-    </row>
-    <row r="12" spans="2:23" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="W11" s="14"/>
+    </row>
+    <row r="12" spans="2:23" ht="25.8" x14ac:dyDescent="0.3">
       <c r="B12" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="43"/>
-      <c r="J12" s="40"/>
-      <c r="W12" s="40"/>
-    </row>
-    <row r="13" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="9"/>
+      <c r="J12" s="14"/>
+      <c r="W12" s="14"/>
+    </row>
+    <row r="13" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="17"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="43"/>
-      <c r="J13" s="40"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="9"/>
+      <c r="J13" s="14"/>
       <c r="L13" s="1"/>
       <c r="M13" s="4"/>
       <c r="O13" s="1"/>
@@ -993,12 +1024,12 @@
         <v>2</v>
       </c>
       <c r="U13" s="23"/>
-      <c r="V13" s="45"/>
-      <c r="W13" s="40"/>
-    </row>
-    <row r="14" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V13" s="10"/>
+      <c r="W13" s="14"/>
+    </row>
+    <row r="14" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I14" s="6"/>
-      <c r="J14" s="40"/>
+      <c r="J14" s="14"/>
       <c r="L14" s="22">
         <v>10</v>
       </c>
@@ -1013,12 +1044,12 @@
       <c r="R14" s="23"/>
       <c r="T14" s="24"/>
       <c r="U14" s="25"/>
-      <c r="V14" s="45"/>
-      <c r="W14" s="40"/>
-    </row>
-    <row r="15" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V14" s="10"/>
+      <c r="W14" s="14"/>
+    </row>
+    <row r="15" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I15" s="6"/>
-      <c r="J15" s="40"/>
+      <c r="J15" s="14"/>
       <c r="L15" s="24"/>
       <c r="M15" s="25"/>
       <c r="O15" s="24"/>
@@ -1027,12 +1058,12 @@
       <c r="R15" s="25"/>
       <c r="T15" s="24"/>
       <c r="U15" s="25"/>
-      <c r="V15" s="45"/>
-      <c r="W15" s="40"/>
-    </row>
-    <row r="16" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V15" s="10"/>
+      <c r="W15" s="14"/>
+    </row>
+    <row r="16" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I16" s="6"/>
-      <c r="J16" s="40"/>
+      <c r="J16" s="14"/>
       <c r="L16" s="26"/>
       <c r="M16" s="27"/>
       <c r="O16" s="24"/>
@@ -1041,12 +1072,12 @@
       <c r="R16" s="25"/>
       <c r="T16" s="24"/>
       <c r="U16" s="25"/>
-      <c r="V16" s="45"/>
-      <c r="W16" s="40"/>
-    </row>
-    <row r="17" spans="5:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V16" s="10"/>
+      <c r="W16" s="14"/>
+    </row>
+    <row r="17" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I17" s="6"/>
-      <c r="J17" s="40"/>
+      <c r="J17" s="14"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="O17" s="24"/>
@@ -1055,34 +1086,38 @@
       <c r="R17" s="25"/>
       <c r="T17" s="26"/>
       <c r="U17" s="27"/>
-      <c r="V17" s="45"/>
-      <c r="W17" s="40"/>
-    </row>
-    <row r="18" spans="5:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I18" s="11" t="s">
+      <c r="V17" s="10"/>
+      <c r="W17" s="14"/>
+    </row>
+    <row r="18" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I18" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="40"/>
-      <c r="L18" s="14" t="s">
+      <c r="J18" s="14"/>
+      <c r="L18" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="M18" s="14"/>
+      <c r="M18" s="28"/>
       <c r="O18" s="24"/>
       <c r="P18" s="25"/>
       <c r="Q18" s="24"/>
       <c r="R18" s="25"/>
-      <c r="T18" s="14" t="s">
+      <c r="T18" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="U18" s="14"/>
-      <c r="V18" s="45"/>
-      <c r="W18" s="40"/>
-      <c r="X18" s="11" t="s">
+      <c r="U18" s="28"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="5:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I19" s="11"/>
+    <row r="19" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="47">
+        <v>13</v>
+      </c>
+      <c r="D19" s="48"/>
+      <c r="I19" s="13"/>
       <c r="L19" s="22">
         <v>11</v>
       </c>
@@ -1093,11 +1128,13 @@
       <c r="R19" s="25"/>
       <c r="T19" s="1"/>
       <c r="U19" s="4"/>
-      <c r="W19" s="42"/>
-      <c r="X19" s="11"/>
-    </row>
-    <row r="20" spans="5:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I20" s="11"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="13"/>
+    </row>
+    <row r="20" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="49"/>
+      <c r="D20" s="50"/>
+      <c r="I20" s="13"/>
       <c r="L20" s="24"/>
       <c r="M20" s="25"/>
       <c r="O20" s="24"/>
@@ -1108,11 +1145,13 @@
         <v>3</v>
       </c>
       <c r="U20" s="23"/>
-      <c r="W20" s="42"/>
-      <c r="X20" s="11"/>
-    </row>
-    <row r="21" spans="5:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I21" s="11"/>
+      <c r="W20" s="8"/>
+      <c r="X20" s="13"/>
+    </row>
+    <row r="21" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="49"/>
+      <c r="D21" s="50"/>
+      <c r="I21" s="13"/>
       <c r="L21" s="24"/>
       <c r="M21" s="25"/>
       <c r="O21" s="24"/>
@@ -1121,11 +1160,13 @@
       <c r="R21" s="25"/>
       <c r="T21" s="24"/>
       <c r="U21" s="25"/>
-      <c r="W21" s="42"/>
-      <c r="X21" s="11"/>
-    </row>
-    <row r="22" spans="5:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I22" s="11"/>
+      <c r="W21" s="8"/>
+      <c r="X21" s="13"/>
+    </row>
+    <row r="22" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="49"/>
+      <c r="D22" s="50"/>
+      <c r="I22" s="13"/>
       <c r="L22" s="24"/>
       <c r="M22" s="25"/>
       <c r="O22" s="24"/>
@@ -1134,11 +1175,13 @@
       <c r="R22" s="25"/>
       <c r="T22" s="26"/>
       <c r="U22" s="27"/>
-      <c r="W22" s="42"/>
-      <c r="X22" s="11"/>
-    </row>
-    <row r="23" spans="5:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I23" s="11"/>
+      <c r="W22" s="8"/>
+      <c r="X22" s="13"/>
+    </row>
+    <row r="23" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="49"/>
+      <c r="D23" s="50"/>
+      <c r="I23" s="13"/>
       <c r="L23" s="26"/>
       <c r="M23" s="27"/>
       <c r="O23" s="26"/>
@@ -1147,40 +1190,44 @@
       <c r="R23" s="27"/>
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
-      <c r="W23" s="42"/>
-      <c r="X23" s="11"/>
-    </row>
-    <row r="24" spans="5:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W23" s="8"/>
+      <c r="X23" s="13"/>
+    </row>
+    <row r="24" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="49"/>
+      <c r="D24" s="50"/>
       <c r="E24" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="44" t="s">
+      <c r="F24" s="12" t="s">
         <v>18</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I24" s="11"/>
-      <c r="L24" s="13" t="s">
+      <c r="I24" s="13"/>
+      <c r="L24" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="M24" s="13"/>
+      <c r="M24" s="42"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
-      <c r="T24" s="13" t="s">
+      <c r="T24" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="U24" s="13"/>
-      <c r="W24" s="42"/>
-      <c r="X24" s="11"/>
-      <c r="Y24" s="44" t="s">
+      <c r="U24" s="42"/>
+      <c r="W24" s="8"/>
+      <c r="X24" s="13"/>
+      <c r="Y24" s="12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="5:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F25" s="44"/>
+    <row r="25" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="49"/>
+      <c r="D25" s="50"/>
+      <c r="F25" s="12"/>
       <c r="H25" s="7"/>
       <c r="L25" s="22">
         <v>12</v>
@@ -1196,11 +1243,13 @@
         <v>4</v>
       </c>
       <c r="U25" s="23"/>
-      <c r="X25" s="46"/>
-      <c r="Y25" s="44"/>
-    </row>
-    <row r="26" spans="5:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F26" s="44"/>
+      <c r="X25" s="11"/>
+      <c r="Y25" s="12"/>
+    </row>
+    <row r="26" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="49"/>
+      <c r="D26" s="50"/>
+      <c r="F26" s="12"/>
       <c r="H26" s="7"/>
       <c r="L26" s="24"/>
       <c r="M26" s="25"/>
@@ -1210,11 +1259,13 @@
       <c r="R26" s="25"/>
       <c r="T26" s="24"/>
       <c r="U26" s="25"/>
-      <c r="X26" s="46"/>
-      <c r="Y26" s="44"/>
-    </row>
-    <row r="27" spans="5:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F27" s="44"/>
+      <c r="X26" s="11"/>
+      <c r="Y26" s="12"/>
+    </row>
+    <row r="27" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="49"/>
+      <c r="D27" s="50"/>
+      <c r="F27" s="12"/>
       <c r="H27" s="7"/>
       <c r="L27" s="24"/>
       <c r="M27" s="25"/>
@@ -1222,11 +1273,13 @@
       <c r="R27" s="25"/>
       <c r="T27" s="24"/>
       <c r="U27" s="25"/>
-      <c r="X27" s="46"/>
-      <c r="Y27" s="44"/>
-    </row>
-    <row r="28" spans="5:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F28" s="44"/>
+      <c r="X27" s="11"/>
+      <c r="Y27" s="12"/>
+    </row>
+    <row r="28" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="49"/>
+      <c r="D28" s="50"/>
+      <c r="F28" s="12"/>
       <c r="H28" s="7"/>
       <c r="L28" s="24"/>
       <c r="M28" s="25"/>
@@ -1234,11 +1287,13 @@
       <c r="R28" s="25"/>
       <c r="T28" s="24"/>
       <c r="U28" s="25"/>
-      <c r="X28" s="46"/>
-      <c r="Y28" s="44"/>
-    </row>
-    <row r="29" spans="5:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F29" s="44"/>
+      <c r="X28" s="11"/>
+      <c r="Y28" s="12"/>
+    </row>
+    <row r="29" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="51"/>
+      <c r="D29" s="52"/>
+      <c r="F29" s="12"/>
       <c r="H29" s="7"/>
       <c r="L29" s="26"/>
       <c r="M29" s="27"/>
@@ -1246,45 +1301,55 @@
       <c r="R29" s="27"/>
       <c r="T29" s="26"/>
       <c r="U29" s="27"/>
-      <c r="X29" s="46"/>
-      <c r="Y29" s="44"/>
-    </row>
-    <row r="30" spans="5:25" x14ac:dyDescent="0.25">
-      <c r="F30" s="44"/>
+      <c r="X29" s="11"/>
+      <c r="Y29" s="12"/>
+    </row>
+    <row r="30" spans="3:25" x14ac:dyDescent="0.3">
+      <c r="F30" s="12"/>
       <c r="H30" s="7"/>
-      <c r="L30" s="15">
+      <c r="L30" s="43">
         <v>3100</v>
       </c>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="15"/>
-      <c r="T30" s="15"/>
-      <c r="U30" s="15"/>
-      <c r="X30" s="46"/>
-      <c r="Y30" s="44"/>
-    </row>
-    <row r="31" spans="5:25" x14ac:dyDescent="0.25">
-      <c r="L31" s="10" t="s">
+      <c r="M30" s="43"/>
+      <c r="N30" s="43"/>
+      <c r="O30" s="43"/>
+      <c r="P30" s="43"/>
+      <c r="Q30" s="43"/>
+      <c r="R30" s="43"/>
+      <c r="S30" s="43"/>
+      <c r="T30" s="43"/>
+      <c r="U30" s="43"/>
+      <c r="X30" s="11"/>
+      <c r="Y30" s="12"/>
+    </row>
+    <row r="31" spans="3:25" x14ac:dyDescent="0.3">
+      <c r="C31" s="53" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="53"/>
+      <c r="E31" s="53"/>
+      <c r="F31" s="53"/>
+      <c r="G31" s="53"/>
+      <c r="H31" s="53"/>
+      <c r="I31" s="53"/>
+      <c r="J31" s="53"/>
+      <c r="L31" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="M31" s="10"/>
-      <c r="O31" s="9" t="s">
+      <c r="M31" s="46"/>
+      <c r="O31" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="P31" s="9"/>
-      <c r="Q31" s="9"/>
-      <c r="R31" s="9"/>
+      <c r="P31" s="45"/>
+      <c r="Q31" s="45"/>
+      <c r="R31" s="45"/>
       <c r="S31" s="3"/>
-      <c r="T31" s="12" t="s">
+      <c r="T31" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="U31" s="12"/>
-    </row>
-    <row r="32" spans="5:25" x14ac:dyDescent="0.25">
+      <c r="U31" s="41"/>
+    </row>
+    <row r="32" spans="3:25" x14ac:dyDescent="0.3">
       <c r="L32" t="s">
         <v>23</v>
       </c>
@@ -1304,17 +1369,17 @@
         <v>9</v>
       </c>
     </row>
-    <row r="33" spans="15:18" x14ac:dyDescent="0.25">
-      <c r="O33" s="8" t="s">
+    <row r="33" spans="15:18" x14ac:dyDescent="0.3">
+      <c r="O33" s="44" t="s">
         <v>12</v>
       </c>
-      <c r="P33" s="8"/>
-      <c r="Q33" s="8" t="s">
+      <c r="P33" s="44"/>
+      <c r="Q33" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="R33" s="8"/>
-    </row>
-    <row r="34" spans="15:18" x14ac:dyDescent="0.25">
+      <c r="R33" s="44"/>
+    </row>
+    <row r="34" spans="15:18" x14ac:dyDescent="0.3">
       <c r="O34" t="s">
         <v>10</v>
       </c>
@@ -1329,28 +1394,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="35">
-    <mergeCell ref="Y24:Y30"/>
-    <mergeCell ref="I18:I24"/>
-    <mergeCell ref="J9:J18"/>
-    <mergeCell ref="F24:F30"/>
-    <mergeCell ref="V5:V10"/>
-    <mergeCell ref="W9:W18"/>
-    <mergeCell ref="K5:K10"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="L14:M16"/>
-    <mergeCell ref="T18:U18"/>
-    <mergeCell ref="L18:M18"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="Q14:R23"/>
-    <mergeCell ref="T13:U17"/>
-    <mergeCell ref="L5:U6"/>
-    <mergeCell ref="M7:T9"/>
-    <mergeCell ref="O14:P23"/>
+  <mergeCells count="37">
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="O31:R31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="C19:D29"/>
+    <mergeCell ref="C31:J31"/>
     <mergeCell ref="T31:U31"/>
     <mergeCell ref="L24:M24"/>
     <mergeCell ref="T24:U24"/>
@@ -1360,11 +1410,28 @@
     <mergeCell ref="Q25:R29"/>
     <mergeCell ref="L19:M23"/>
     <mergeCell ref="L25:M29"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="L14:M16"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="L5:U6"/>
+    <mergeCell ref="M7:T9"/>
+    <mergeCell ref="O14:P23"/>
+    <mergeCell ref="Y24:Y30"/>
+    <mergeCell ref="I18:I24"/>
+    <mergeCell ref="J9:J18"/>
+    <mergeCell ref="F24:F30"/>
+    <mergeCell ref="V5:V10"/>
+    <mergeCell ref="W9:W18"/>
+    <mergeCell ref="K5:K10"/>
+    <mergeCell ref="T18:U18"/>
+    <mergeCell ref="L18:M18"/>
+    <mergeCell ref="Q14:R23"/>
+    <mergeCell ref="T13:U17"/>
     <mergeCell ref="X18:X24"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="O31:R31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="O33:P33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Change the layout and add Compass
</commit_message>
<xml_diff>
--- a/Objek/denah palgading.xlsx
+++ b/Objek/denah palgading.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Kasir</t>
   </si>
@@ -102,13 +102,22 @@
   </si>
   <si>
     <t>9526 - 9471</t>
+  </si>
+  <si>
+    <t>Longitude = 110.410XXX</t>
+  </si>
+  <si>
+    <t>Latitude = -7.728XXX</t>
+  </si>
+  <si>
+    <t>[410]9526</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,8 +160,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,8 +251,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -405,11 +443,46 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -438,6 +511,108 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" textRotation="180"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
@@ -450,118 +625,38 @@
     <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -584,6 +679,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>497283</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>250864</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209300</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>112318</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Compass Stock Illustration - Download Image Now - iStock"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="5400000">
+          <a:off x="803564" y="415637"/>
+          <a:ext cx="2133600" cy="2164272"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -849,10 +1004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:Y34"/>
+  <dimension ref="C2:AE34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J35" sqref="J35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -876,111 +1031,146 @@
     <col min="26" max="26" width="9.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:23" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K5" s="15" t="s">
+    <row r="2" spans="3:31" ht="21" x14ac:dyDescent="0.3">
+      <c r="C2" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="52"/>
+      <c r="R2" s="52"/>
+      <c r="S2" s="52"/>
+      <c r="T2" s="52"/>
+      <c r="U2" s="52"/>
+      <c r="V2" s="52"/>
+      <c r="W2" s="52"/>
+      <c r="X2" s="52"/>
+      <c r="Y2" s="52"/>
+    </row>
+    <row r="4" spans="3:31" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="3:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K5" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="33" t="s">
+      <c r="L5" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="34"/>
-      <c r="N5" s="34"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="34"/>
-      <c r="Q5" s="34"/>
-      <c r="R5" s="34"/>
-      <c r="S5" s="34"/>
-      <c r="T5" s="34"/>
-      <c r="U5" s="35"/>
-      <c r="V5" s="15" t="s">
+      <c r="M5" s="39"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="39"/>
+      <c r="P5" s="39"/>
+      <c r="Q5" s="39"/>
+      <c r="R5" s="39"/>
+      <c r="S5" s="39"/>
+      <c r="T5" s="39"/>
+      <c r="U5" s="40"/>
+      <c r="V5" s="49" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="6" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C6" s="18" t="s">
+      <c r="AA5" s="54" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD5" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="15"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="37"/>
-      <c r="N6" s="37"/>
-      <c r="O6" s="37"/>
-      <c r="P6" s="37"/>
-      <c r="Q6" s="37"/>
-      <c r="R6" s="37"/>
-      <c r="S6" s="37"/>
-      <c r="T6" s="37"/>
-      <c r="U6" s="38"/>
-      <c r="V6" s="15"/>
-    </row>
-    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C7" s="19"/>
-      <c r="K7" s="15"/>
-      <c r="M7" s="24">
+    </row>
+    <row r="6" spans="3:31" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K6" s="49"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="42"/>
+      <c r="P6" s="42"/>
+      <c r="Q6" s="42"/>
+      <c r="R6" s="42"/>
+      <c r="S6" s="42"/>
+      <c r="T6" s="42"/>
+      <c r="U6" s="43"/>
+      <c r="V6" s="49"/>
+      <c r="AA6" s="54"/>
+      <c r="AD6" s="33"/>
+    </row>
+    <row r="7" spans="3:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K7" s="49"/>
+      <c r="M7" s="55">
         <v>1</v>
       </c>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="39"/>
-      <c r="Q7" s="39"/>
-      <c r="R7" s="39"/>
-      <c r="S7" s="39"/>
-      <c r="T7" s="25"/>
-      <c r="V7" s="15"/>
-    </row>
-    <row r="8" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C8" s="20" t="s">
+      <c r="N7" s="56"/>
+      <c r="O7" s="56"/>
+      <c r="P7" s="56"/>
+      <c r="Q7" s="56"/>
+      <c r="R7" s="56"/>
+      <c r="S7" s="56"/>
+      <c r="T7" s="57"/>
+      <c r="V7" s="49"/>
+      <c r="AA7" s="54"/>
+      <c r="AD7" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="K8" s="15"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="39"/>
-      <c r="Q8" s="39"/>
-      <c r="R8" s="39"/>
-      <c r="S8" s="39"/>
-      <c r="T8" s="25"/>
-      <c r="V8" s="15"/>
-    </row>
-    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
-      <c r="C9" s="21"/>
-      <c r="J9" s="14" t="s">
+    </row>
+    <row r="8" spans="3:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K8" s="49"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="44"/>
+      <c r="P8" s="44"/>
+      <c r="Q8" s="44"/>
+      <c r="R8" s="44"/>
+      <c r="S8" s="44"/>
+      <c r="T8" s="29"/>
+      <c r="V8" s="49"/>
+      <c r="AA8" s="54"/>
+      <c r="AD8" s="34"/>
+    </row>
+    <row r="9" spans="3:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="15"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="40"/>
-      <c r="O9" s="40"/>
-      <c r="P9" s="40"/>
-      <c r="Q9" s="40"/>
-      <c r="R9" s="40"/>
-      <c r="S9" s="40"/>
-      <c r="T9" s="27"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="14" t="s">
+      <c r="K9" s="49"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="45"/>
+      <c r="O9" s="45"/>
+      <c r="P9" s="45"/>
+      <c r="Q9" s="45"/>
+      <c r="R9" s="45"/>
+      <c r="S9" s="45"/>
+      <c r="T9" s="31"/>
+      <c r="V9" s="49"/>
+      <c r="W9" s="48" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="19" t="s">
+      <c r="AA9" s="54"/>
+      <c r="AD9" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="J10" s="14"/>
-      <c r="K10" s="15"/>
+    </row>
+    <row r="10" spans="3:31" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J10" s="48"/>
+      <c r="K10" s="49"/>
       <c r="L10" t="s">
         <v>16</v>
       </c>
       <c r="U10" t="s">
         <v>16</v>
       </c>
-      <c r="V10" s="15"/>
-      <c r="W10" s="14"/>
-    </row>
-    <row r="11" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C11" s="19"/>
-      <c r="J11" s="14"/>
+      <c r="V10" s="49"/>
+      <c r="W10" s="48"/>
+      <c r="AA10" s="54"/>
+      <c r="AD10" s="59"/>
+    </row>
+    <row r="11" spans="3:31" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="J11" s="48"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -992,364 +1182,397 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="3"/>
-      <c r="W11" s="14"/>
-    </row>
-    <row r="12" spans="2:23" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="B12" s="16" t="s">
+      <c r="W11" s="48"/>
+      <c r="AA11" s="54"/>
+      <c r="AC11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="AD11" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="31" t="s">
+      <c r="AE11" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="9"/>
-      <c r="J12" s="14"/>
-      <c r="W12" s="14"/>
-    </row>
-    <row r="13" spans="2:23" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="17"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="32"/>
-      <c r="E13" s="9"/>
-      <c r="J13" s="14"/>
+    </row>
+    <row r="12" spans="3:31" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="J12" s="48"/>
+      <c r="W12" s="48"/>
+      <c r="AA12" s="54"/>
+      <c r="AC12" s="13"/>
+      <c r="AD12" s="58"/>
+      <c r="AE12" s="37"/>
+    </row>
+    <row r="13" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J13" s="48"/>
       <c r="L13" s="1"/>
       <c r="M13" s="4"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
-      <c r="T13" s="22">
+      <c r="T13" s="26">
         <v>2</v>
       </c>
-      <c r="U13" s="23"/>
+      <c r="U13" s="27"/>
       <c r="V13" s="10"/>
-      <c r="W13" s="14"/>
-    </row>
-    <row r="14" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W13" s="48"/>
+      <c r="AA13" s="54"/>
+    </row>
+    <row r="14" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I14" s="6"/>
-      <c r="J14" s="14"/>
-      <c r="L14" s="22">
+      <c r="J14" s="48"/>
+      <c r="L14" s="26">
         <v>10</v>
       </c>
-      <c r="M14" s="23"/>
-      <c r="O14" s="22">
+      <c r="M14" s="27"/>
+      <c r="O14" s="26">
         <v>9</v>
       </c>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="22">
+      <c r="P14" s="27"/>
+      <c r="Q14" s="26">
         <v>6</v>
       </c>
-      <c r="R14" s="23"/>
-      <c r="T14" s="24"/>
-      <c r="U14" s="25"/>
+      <c r="R14" s="27"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="29"/>
       <c r="V14" s="10"/>
-      <c r="W14" s="14"/>
-    </row>
-    <row r="15" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W14" s="48"/>
+      <c r="AA14" s="54"/>
+    </row>
+    <row r="15" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I15" s="6"/>
-      <c r="J15" s="14"/>
-      <c r="L15" s="24"/>
-      <c r="M15" s="25"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="25"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="25"/>
+      <c r="J15" s="48"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="29"/>
+      <c r="O15" s="28"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="29"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="29"/>
       <c r="V15" s="10"/>
-      <c r="W15" s="14"/>
-    </row>
-    <row r="16" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W15" s="48"/>
+      <c r="AA15" s="54"/>
+    </row>
+    <row r="16" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I16" s="6"/>
-      <c r="J16" s="14"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="27"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="25"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="25"/>
+      <c r="J16" s="48"/>
+      <c r="L16" s="30"/>
+      <c r="M16" s="31"/>
+      <c r="O16" s="28"/>
+      <c r="P16" s="29"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="29"/>
+      <c r="T16" s="28"/>
+      <c r="U16" s="29"/>
       <c r="V16" s="10"/>
-      <c r="W16" s="14"/>
-    </row>
-    <row r="17" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="W16" s="48"/>
+      <c r="AA16" s="54"/>
+    </row>
+    <row r="17" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I17" s="6"/>
-      <c r="J17" s="14"/>
+      <c r="J17" s="48"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="25"/>
-      <c r="T17" s="26"/>
-      <c r="U17" s="27"/>
+      <c r="O17" s="28"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="29"/>
+      <c r="T17" s="28"/>
+      <c r="U17" s="29"/>
       <c r="V17" s="10"/>
-      <c r="W17" s="14"/>
-    </row>
-    <row r="18" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I18" s="13" t="s">
+      <c r="W17" s="48"/>
+      <c r="AA17" s="54"/>
+    </row>
+    <row r="18" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I18" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="14"/>
-      <c r="L18" s="28" t="s">
+      <c r="J18" s="48"/>
+      <c r="L18" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="M18" s="28"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="25"/>
-      <c r="T18" s="28" t="s">
+      <c r="M18" s="50"/>
+      <c r="O18" s="28"/>
+      <c r="P18" s="29"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="29"/>
+      <c r="T18" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="U18" s="28"/>
+      <c r="U18" s="60"/>
       <c r="V18" s="10"/>
-      <c r="W18" s="14"/>
-      <c r="X18" s="13" t="s">
+      <c r="W18" s="48"/>
+      <c r="X18" s="47" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="47">
+      <c r="AA18" s="54"/>
+      <c r="AE18" s="9"/>
+    </row>
+    <row r="19" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="17">
         <v>13</v>
       </c>
-      <c r="D19" s="48"/>
-      <c r="I19" s="13"/>
-      <c r="L19" s="22">
+      <c r="D19" s="18"/>
+      <c r="I19" s="47"/>
+      <c r="L19" s="26">
         <v>11</v>
       </c>
-      <c r="M19" s="23"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="25"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="25"/>
+      <c r="M19" s="27"/>
+      <c r="O19" s="28"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="29"/>
       <c r="T19" s="1"/>
       <c r="U19" s="4"/>
       <c r="W19" s="8"/>
-      <c r="X19" s="13"/>
-    </row>
-    <row r="20" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="49"/>
-      <c r="D20" s="50"/>
-      <c r="I20" s="13"/>
-      <c r="L20" s="24"/>
-      <c r="M20" s="25"/>
-      <c r="O20" s="24"/>
-      <c r="P20" s="25"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="25"/>
-      <c r="T20" s="22">
+      <c r="X19" s="47"/>
+      <c r="AA19" s="54"/>
+      <c r="AE19" s="9"/>
+    </row>
+    <row r="20" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="19"/>
+      <c r="D20" s="20"/>
+      <c r="I20" s="47"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="29"/>
+      <c r="O20" s="28"/>
+      <c r="P20" s="29"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="29"/>
+      <c r="T20" s="26">
         <v>3</v>
       </c>
-      <c r="U20" s="23"/>
+      <c r="U20" s="27"/>
       <c r="W20" s="8"/>
-      <c r="X20" s="13"/>
-    </row>
-    <row r="21" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="49"/>
-      <c r="D21" s="50"/>
-      <c r="I21" s="13"/>
-      <c r="L21" s="24"/>
-      <c r="M21" s="25"/>
-      <c r="O21" s="24"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="25"/>
-      <c r="T21" s="24"/>
-      <c r="U21" s="25"/>
+      <c r="X20" s="47"/>
+      <c r="AA20" s="54"/>
+    </row>
+    <row r="21" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="19"/>
+      <c r="D21" s="20"/>
+      <c r="I21" s="47"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="29"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="29"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="29"/>
+      <c r="T21" s="28"/>
+      <c r="U21" s="29"/>
       <c r="W21" s="8"/>
-      <c r="X21" s="13"/>
-    </row>
-    <row r="22" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="49"/>
-      <c r="D22" s="50"/>
-      <c r="I22" s="13"/>
-      <c r="L22" s="24"/>
-      <c r="M22" s="25"/>
-      <c r="O22" s="24"/>
-      <c r="P22" s="25"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="25"/>
-      <c r="T22" s="26"/>
-      <c r="U22" s="27"/>
+      <c r="X21" s="47"/>
+      <c r="AA21" s="54"/>
+    </row>
+    <row r="22" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="I22" s="47"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="29"/>
+      <c r="O22" s="28"/>
+      <c r="P22" s="29"/>
+      <c r="Q22" s="28"/>
+      <c r="R22" s="29"/>
+      <c r="T22" s="28"/>
+      <c r="U22" s="29"/>
       <c r="W22" s="8"/>
-      <c r="X22" s="13"/>
-    </row>
-    <row r="23" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="49"/>
-      <c r="D23" s="50"/>
-      <c r="I23" s="13"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="27"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="26"/>
-      <c r="R23" s="27"/>
+      <c r="X22" s="47"/>
+      <c r="AA22" s="54"/>
+    </row>
+    <row r="23" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="19"/>
+      <c r="D23" s="20"/>
+      <c r="I23" s="47"/>
+      <c r="L23" s="30"/>
+      <c r="M23" s="31"/>
+      <c r="O23" s="30"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="30"/>
+      <c r="R23" s="31"/>
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
       <c r="W23" s="8"/>
-      <c r="X23" s="13"/>
-    </row>
-    <row r="24" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="49"/>
-      <c r="D24" s="50"/>
+      <c r="X23" s="47"/>
+      <c r="AA23" s="54"/>
+    </row>
+    <row r="24" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="19"/>
+      <c r="D24" s="20"/>
       <c r="E24" t="s">
         <v>17</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="F24" s="46" t="s">
         <v>18</v>
       </c>
       <c r="H24" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I24" s="13"/>
-      <c r="L24" s="42" t="s">
+      <c r="I24" s="47"/>
+      <c r="L24" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="M24" s="42"/>
+      <c r="M24" s="24"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
-      <c r="T24" s="42" t="s">
+      <c r="T24" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="U24" s="42"/>
+      <c r="U24" s="50"/>
       <c r="W24" s="8"/>
-      <c r="X24" s="13"/>
-      <c r="Y24" s="12" t="s">
+      <c r="X24" s="47"/>
+      <c r="Y24" s="46" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="49"/>
-      <c r="D25" s="50"/>
-      <c r="F25" s="12"/>
+      <c r="AA24" s="54"/>
+      <c r="AB24" s="53"/>
+      <c r="AC24" s="53"/>
+    </row>
+    <row r="25" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="19"/>
+      <c r="D25" s="20"/>
+      <c r="F25" s="46"/>
       <c r="H25" s="7"/>
-      <c r="L25" s="22">
+      <c r="L25" s="26">
         <v>12</v>
       </c>
-      <c r="M25" s="23"/>
+      <c r="M25" s="27"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
-      <c r="Q25" s="22">
+      <c r="Q25" s="26">
         <v>7</v>
       </c>
-      <c r="R25" s="23"/>
-      <c r="T25" s="22">
+      <c r="R25" s="27"/>
+      <c r="T25" s="26">
         <v>4</v>
       </c>
-      <c r="U25" s="23"/>
+      <c r="U25" s="27"/>
       <c r="X25" s="11"/>
-      <c r="Y25" s="12"/>
-    </row>
-    <row r="26" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="49"/>
-      <c r="D26" s="50"/>
-      <c r="F26" s="12"/>
+      <c r="Y25" s="46"/>
+      <c r="AA25" s="54"/>
+    </row>
+    <row r="26" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="19"/>
+      <c r="D26" s="20"/>
+      <c r="F26" s="46"/>
       <c r="H26" s="7"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="25"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="29"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
-      <c r="Q26" s="24"/>
-      <c r="R26" s="25"/>
-      <c r="T26" s="24"/>
-      <c r="U26" s="25"/>
+      <c r="Q26" s="28"/>
+      <c r="R26" s="29"/>
+      <c r="T26" s="28"/>
+      <c r="U26" s="29"/>
       <c r="X26" s="11"/>
-      <c r="Y26" s="12"/>
-    </row>
-    <row r="27" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="49"/>
-      <c r="D27" s="50"/>
-      <c r="F27" s="12"/>
+      <c r="Y26" s="46"/>
+      <c r="AA26" s="54"/>
+    </row>
+    <row r="27" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="19"/>
+      <c r="D27" s="20"/>
+      <c r="F27" s="46"/>
       <c r="H27" s="7"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="25"/>
-      <c r="Q27" s="24"/>
-      <c r="R27" s="25"/>
-      <c r="T27" s="24"/>
-      <c r="U27" s="25"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="29"/>
+      <c r="Q27" s="28"/>
+      <c r="R27" s="29"/>
+      <c r="T27" s="28"/>
+      <c r="U27" s="29"/>
       <c r="X27" s="11"/>
-      <c r="Y27" s="12"/>
-    </row>
-    <row r="28" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="49"/>
-      <c r="D28" s="50"/>
-      <c r="F28" s="12"/>
+      <c r="Y27" s="46"/>
+      <c r="AA27" s="54"/>
+    </row>
+    <row r="28" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="19"/>
+      <c r="D28" s="20"/>
+      <c r="F28" s="46"/>
       <c r="H28" s="7"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="25"/>
-      <c r="Q28" s="24"/>
-      <c r="R28" s="25"/>
-      <c r="T28" s="24"/>
-      <c r="U28" s="25"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="29"/>
+      <c r="Q28" s="28"/>
+      <c r="R28" s="29"/>
+      <c r="T28" s="28"/>
+      <c r="U28" s="29"/>
       <c r="X28" s="11"/>
-      <c r="Y28" s="12"/>
-    </row>
-    <row r="29" spans="3:25" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="51"/>
-      <c r="D29" s="52"/>
-      <c r="F29" s="12"/>
+      <c r="Y28" s="46"/>
+      <c r="AA28" s="54"/>
+    </row>
+    <row r="29" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="21"/>
+      <c r="D29" s="22"/>
+      <c r="F29" s="46"/>
       <c r="H29" s="7"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="27"/>
-      <c r="Q29" s="26"/>
-      <c r="R29" s="27"/>
-      <c r="T29" s="26"/>
-      <c r="U29" s="27"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="31"/>
+      <c r="Q29" s="30"/>
+      <c r="R29" s="31"/>
+      <c r="T29" s="30"/>
+      <c r="U29" s="31"/>
       <c r="X29" s="11"/>
-      <c r="Y29" s="12"/>
-    </row>
-    <row r="30" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="F30" s="12"/>
+      <c r="Y29" s="46"/>
+      <c r="AA29" s="54"/>
+    </row>
+    <row r="30" spans="3:31" x14ac:dyDescent="0.3">
+      <c r="F30" s="46"/>
       <c r="H30" s="7"/>
-      <c r="L30" s="43">
+      <c r="L30" s="25">
         <v>3100</v>
       </c>
-      <c r="M30" s="43"/>
-      <c r="N30" s="43"/>
-      <c r="O30" s="43"/>
-      <c r="P30" s="43"/>
-      <c r="Q30" s="43"/>
-      <c r="R30" s="43"/>
-      <c r="S30" s="43"/>
-      <c r="T30" s="43"/>
-      <c r="U30" s="43"/>
+      <c r="M30" s="25"/>
+      <c r="N30" s="25"/>
+      <c r="O30" s="25"/>
+      <c r="P30" s="25"/>
+      <c r="Q30" s="25"/>
+      <c r="R30" s="25"/>
+      <c r="S30" s="25"/>
+      <c r="T30" s="25"/>
+      <c r="U30" s="25"/>
       <c r="X30" s="11"/>
-      <c r="Y30" s="12"/>
-    </row>
-    <row r="31" spans="3:25" x14ac:dyDescent="0.3">
-      <c r="C31" s="53" t="s">
+      <c r="Y30" s="46"/>
+      <c r="AA30" s="54"/>
+    </row>
+    <row r="31" spans="3:31" x14ac:dyDescent="0.3">
+      <c r="C31" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-      <c r="F31" s="53"/>
-      <c r="G31" s="53"/>
-      <c r="H31" s="53"/>
-      <c r="I31" s="53"/>
-      <c r="J31" s="53"/>
-      <c r="L31" s="46" t="s">
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="61"/>
+      <c r="L31" s="16" t="s">
         <v>22</v>
       </c>
-      <c r="M31" s="46"/>
-      <c r="O31" s="45" t="s">
+      <c r="M31" s="16"/>
+      <c r="O31" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="P31" s="45"/>
-      <c r="Q31" s="45"/>
-      <c r="R31" s="45"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
       <c r="S31" s="3"/>
-      <c r="T31" s="41" t="s">
+      <c r="T31" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="U31" s="41"/>
-    </row>
-    <row r="32" spans="3:25" x14ac:dyDescent="0.3">
+      <c r="U31" s="23"/>
+      <c r="AA31" s="54"/>
+    </row>
+    <row r="32" spans="3:31" x14ac:dyDescent="0.3">
+      <c r="C32" t="s">
+        <v>28</v>
+      </c>
+      <c r="F32" s="51" t="s">
+        <v>23</v>
+      </c>
+      <c r="G32" s="51"/>
+      <c r="H32" s="51"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="51"/>
       <c r="L32" t="s">
         <v>23</v>
       </c>
@@ -1368,18 +1591,20 @@
       <c r="U32" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="33" spans="15:18" x14ac:dyDescent="0.3">
-      <c r="O33" s="44" t="s">
+      <c r="AA32" s="54"/>
+    </row>
+    <row r="33" spans="15:27" x14ac:dyDescent="0.3">
+      <c r="O33" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="P33" s="44"/>
-      <c r="Q33" s="44" t="s">
+      <c r="P33" s="14"/>
+      <c r="Q33" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="R33" s="44"/>
-    </row>
-    <row r="34" spans="15:18" x14ac:dyDescent="0.3">
+      <c r="R33" s="14"/>
+      <c r="AA33" s="54"/>
+    </row>
+    <row r="34" spans="15:27" x14ac:dyDescent="0.3">
       <c r="O34" t="s">
         <v>10</v>
       </c>
@@ -1392,34 +1617,12 @@
       <c r="R34" t="s">
         <v>8</v>
       </c>
+      <c r="AA34" s="54"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="O31:R31"/>
-    <mergeCell ref="L31:M31"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="C19:D29"/>
-    <mergeCell ref="C31:J31"/>
-    <mergeCell ref="T31:U31"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="L30:U30"/>
-    <mergeCell ref="T20:U22"/>
-    <mergeCell ref="T25:U29"/>
-    <mergeCell ref="Q25:R29"/>
-    <mergeCell ref="L19:M23"/>
-    <mergeCell ref="L25:M29"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="L14:M16"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="L5:U6"/>
-    <mergeCell ref="M7:T9"/>
-    <mergeCell ref="O14:P23"/>
+  <mergeCells count="39">
+    <mergeCell ref="AA5:AA34"/>
+    <mergeCell ref="C2:Y2"/>
     <mergeCell ref="Y24:Y30"/>
     <mergeCell ref="I18:I24"/>
     <mergeCell ref="J9:J18"/>
@@ -1432,8 +1635,34 @@
     <mergeCell ref="Q14:R23"/>
     <mergeCell ref="T13:U17"/>
     <mergeCell ref="X18:X24"/>
+    <mergeCell ref="AD5:AD6"/>
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="L14:M16"/>
+    <mergeCell ref="AD11:AD12"/>
+    <mergeCell ref="AE11:AE12"/>
+    <mergeCell ref="L5:U6"/>
+    <mergeCell ref="M7:T9"/>
+    <mergeCell ref="O14:P23"/>
+    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="L30:U30"/>
+    <mergeCell ref="T20:U22"/>
+    <mergeCell ref="T25:U29"/>
+    <mergeCell ref="Q25:R29"/>
+    <mergeCell ref="L19:M23"/>
+    <mergeCell ref="L25:M29"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="O31:R31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="C19:D29"/>
+    <mergeCell ref="C31:J31"/>
+    <mergeCell ref="F32:J32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Corecting Coordinate on Mapping Table
</commit_message>
<xml_diff>
--- a/Objek/denah palgading.xlsx
+++ b/Objek/denah palgading.xlsx
@@ -41,15 +41,9 @@
     <t>-</t>
   </si>
   <si>
-    <t>3145 - 3110</t>
-  </si>
-  <si>
     <t>[728]3145</t>
   </si>
   <si>
-    <t>[728]3110</t>
-  </si>
-  <si>
     <t>[410]9404</t>
   </si>
   <si>
@@ -59,12 +53,6 @@
     <t>[410]9444</t>
   </si>
   <si>
-    <t>[410]9420</t>
-  </si>
-  <si>
-    <t>9444 - 9420</t>
-  </si>
-  <si>
     <t>3180 - 3163</t>
   </si>
   <si>
@@ -80,9 +68,6 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>3110 - 3100</t>
-  </si>
-  <si>
     <t>9390 - 9377</t>
   </si>
   <si>
@@ -98,9 +83,6 @@
     <t>[410]9471</t>
   </si>
   <si>
-    <t>9420 - 9390</t>
-  </si>
-  <si>
     <t>9526 - 9471</t>
   </si>
   <si>
@@ -111,6 +93,24 @@
   </si>
   <si>
     <t>[410]9526</t>
+  </si>
+  <si>
+    <t>9416 - 9390</t>
+  </si>
+  <si>
+    <t>[410]9416</t>
+  </si>
+  <si>
+    <t>9444 - 9416</t>
+  </si>
+  <si>
+    <t>3145 - 3115</t>
+  </si>
+  <si>
+    <t>[728]3115</t>
+  </si>
+  <si>
+    <t>3115 - 3070</t>
   </si>
 </sst>
 </file>
@@ -517,146 +517,146 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1006,8 +1006,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:AE34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:AA36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1032,145 +1032,145 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:31" ht="21" x14ac:dyDescent="0.3">
-      <c r="C2" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="52"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="52"/>
-      <c r="O2" s="52"/>
-      <c r="P2" s="52"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="52"/>
-      <c r="V2" s="52"/>
-      <c r="W2" s="52"/>
-      <c r="X2" s="52"/>
-      <c r="Y2" s="52"/>
+      <c r="C2" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
     </row>
     <row r="4" spans="3:31" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="3:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K5" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="L5" s="38" t="s">
+      <c r="K5" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="39"/>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="39"/>
-      <c r="T5" s="39"/>
-      <c r="U5" s="40"/>
-      <c r="V5" s="49" t="s">
-        <v>13</v>
-      </c>
-      <c r="AA5" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="AD5" s="32" t="s">
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="38"/>
+      <c r="Q5" s="38"/>
+      <c r="R5" s="38"/>
+      <c r="S5" s="38"/>
+      <c r="T5" s="38"/>
+      <c r="U5" s="39"/>
+      <c r="V5" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA5" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD5" s="29" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="3:31" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="K6" s="49"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
-      <c r="Q6" s="42"/>
-      <c r="R6" s="42"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="43"/>
-      <c r="V6" s="49"/>
-      <c r="AA6" s="54"/>
-      <c r="AD6" s="33"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
+      <c r="U6" s="42"/>
+      <c r="V6" s="20"/>
+      <c r="AA6" s="15"/>
+      <c r="AD6" s="30"/>
     </row>
     <row r="7" spans="3:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K7" s="49"/>
-      <c r="M7" s="55">
+      <c r="K7" s="20"/>
+      <c r="M7" s="43">
         <v>1</v>
       </c>
-      <c r="N7" s="56"/>
-      <c r="O7" s="56"/>
-      <c r="P7" s="56"/>
-      <c r="Q7" s="56"/>
-      <c r="R7" s="56"/>
-      <c r="S7" s="56"/>
-      <c r="T7" s="57"/>
-      <c r="V7" s="49"/>
-      <c r="AA7" s="54"/>
-      <c r="AD7" s="34" t="s">
+      <c r="N7" s="44"/>
+      <c r="O7" s="44"/>
+      <c r="P7" s="44"/>
+      <c r="Q7" s="44"/>
+      <c r="R7" s="44"/>
+      <c r="S7" s="44"/>
+      <c r="T7" s="45"/>
+      <c r="V7" s="20"/>
+      <c r="AA7" s="15"/>
+      <c r="AD7" s="31" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="3:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="K8" s="49"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="44"/>
-      <c r="O8" s="44"/>
-      <c r="P8" s="44"/>
-      <c r="Q8" s="44"/>
-      <c r="R8" s="44"/>
-      <c r="S8" s="44"/>
-      <c r="T8" s="29"/>
-      <c r="V8" s="49"/>
-      <c r="AA8" s="54"/>
-      <c r="AD8" s="34"/>
+      <c r="K8" s="20"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="46"/>
+      <c r="P8" s="46"/>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="46"/>
+      <c r="S8" s="46"/>
+      <c r="T8" s="26"/>
+      <c r="V8" s="20"/>
+      <c r="AA8" s="15"/>
+      <c r="AD8" s="31"/>
     </row>
     <row r="9" spans="3:31" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J9" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="K9" s="49"/>
-      <c r="M9" s="30"/>
-      <c r="N9" s="45"/>
-      <c r="O9" s="45"/>
-      <c r="P9" s="45"/>
-      <c r="Q9" s="45"/>
-      <c r="R9" s="45"/>
-      <c r="S9" s="45"/>
-      <c r="T9" s="31"/>
-      <c r="V9" s="49"/>
-      <c r="W9" s="48" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA9" s="54"/>
-      <c r="AD9" s="33" t="s">
+      <c r="J9" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="K9" s="20"/>
+      <c r="M9" s="27"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
+      <c r="P9" s="47"/>
+      <c r="Q9" s="47"/>
+      <c r="R9" s="47"/>
+      <c r="S9" s="47"/>
+      <c r="T9" s="28"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA9" s="15"/>
+      <c r="AD9" s="30" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="3:31" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J10" s="48"/>
-      <c r="K10" s="49"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
       <c r="L10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="U10" t="s">
-        <v>16</v>
-      </c>
-      <c r="V10" s="49"/>
-      <c r="W10" s="48"/>
-      <c r="AA10" s="54"/>
-      <c r="AD10" s="59"/>
+        <v>12</v>
+      </c>
+      <c r="V10" s="20"/>
+      <c r="W10" s="19"/>
+      <c r="AA10" s="15"/>
+      <c r="AD10" s="32"/>
     </row>
     <row r="11" spans="3:31" ht="25.8" x14ac:dyDescent="0.3">
-      <c r="J11" s="48"/>
+      <c r="J11" s="19"/>
       <c r="L11" s="2"/>
       <c r="M11" s="2"/>
       <c r="N11" s="2"/>
@@ -1182,445 +1182,468 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
       <c r="V11" s="3"/>
-      <c r="W11" s="48"/>
-      <c r="AA11" s="54"/>
+      <c r="W11" s="19"/>
+      <c r="AA11" s="15"/>
       <c r="AC11" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="AD11" s="35" t="s">
+      <c r="AD11" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="AE11" s="36" t="s">
+      <c r="AE11" s="35" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="3:31" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J12" s="48"/>
-      <c r="W12" s="48"/>
-      <c r="AA12" s="54"/>
+      <c r="J12" s="19"/>
+      <c r="W12" s="19"/>
+      <c r="AA12" s="15"/>
       <c r="AC12" s="13"/>
-      <c r="AD12" s="58"/>
-      <c r="AE12" s="37"/>
+      <c r="AD12" s="34"/>
+      <c r="AE12" s="36"/>
     </row>
     <row r="13" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="J13" s="48"/>
+      <c r="J13" s="19"/>
       <c r="L13" s="1"/>
       <c r="M13" s="4"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
-      <c r="T13" s="26">
+      <c r="T13" s="23">
         <v>2</v>
       </c>
-      <c r="U13" s="27"/>
+      <c r="U13" s="24"/>
       <c r="V13" s="10"/>
-      <c r="W13" s="48"/>
-      <c r="AA13" s="54"/>
+      <c r="W13" s="19"/>
+      <c r="AA13" s="15"/>
     </row>
     <row r="14" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I14" s="6"/>
-      <c r="J14" s="48"/>
-      <c r="L14" s="26">
+      <c r="J14" s="19"/>
+      <c r="L14" s="23">
         <v>10</v>
       </c>
-      <c r="M14" s="27"/>
-      <c r="O14" s="26">
+      <c r="M14" s="24"/>
+      <c r="O14" s="23">
         <v>9</v>
       </c>
-      <c r="P14" s="27"/>
-      <c r="Q14" s="26">
+      <c r="P14" s="24"/>
+      <c r="Q14" s="23">
         <v>6</v>
       </c>
-      <c r="R14" s="27"/>
-      <c r="T14" s="28"/>
-      <c r="U14" s="29"/>
+      <c r="R14" s="24"/>
+      <c r="T14" s="25"/>
+      <c r="U14" s="26"/>
       <c r="V14" s="10"/>
-      <c r="W14" s="48"/>
-      <c r="AA14" s="54"/>
+      <c r="W14" s="19"/>
+      <c r="AA14" s="15"/>
     </row>
     <row r="15" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I15" s="6"/>
-      <c r="J15" s="48"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="29"/>
-      <c r="O15" s="28"/>
-      <c r="P15" s="29"/>
-      <c r="Q15" s="28"/>
-      <c r="R15" s="29"/>
-      <c r="T15" s="28"/>
-      <c r="U15" s="29"/>
+      <c r="J15" s="19"/>
+      <c r="L15" s="25"/>
+      <c r="M15" s="26"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="26"/>
+      <c r="Q15" s="25"/>
+      <c r="R15" s="26"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="26"/>
       <c r="V15" s="10"/>
-      <c r="W15" s="48"/>
-      <c r="AA15" s="54"/>
+      <c r="W15" s="19"/>
+      <c r="AA15" s="15"/>
     </row>
     <row r="16" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I16" s="6"/>
-      <c r="J16" s="48"/>
-      <c r="L16" s="30"/>
-      <c r="M16" s="31"/>
-      <c r="O16" s="28"/>
-      <c r="P16" s="29"/>
-      <c r="Q16" s="28"/>
-      <c r="R16" s="29"/>
-      <c r="T16" s="28"/>
-      <c r="U16" s="29"/>
+      <c r="J16" s="19"/>
+      <c r="L16" s="27"/>
+      <c r="M16" s="28"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="26"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="26"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="26"/>
       <c r="V16" s="10"/>
-      <c r="W16" s="48"/>
-      <c r="AA16" s="54"/>
+      <c r="W16" s="19"/>
+      <c r="AA16" s="15"/>
     </row>
     <row r="17" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I17" s="6"/>
-      <c r="J17" s="48"/>
+      <c r="J17" s="19"/>
       <c r="L17" s="4"/>
       <c r="M17" s="4"/>
-      <c r="O17" s="28"/>
-      <c r="P17" s="29"/>
-      <c r="Q17" s="28"/>
-      <c r="R17" s="29"/>
-      <c r="T17" s="28"/>
-      <c r="U17" s="29"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="26"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="26"/>
       <c r="V17" s="10"/>
-      <c r="W17" s="48"/>
-      <c r="AA17" s="54"/>
+      <c r="W17" s="19"/>
+      <c r="AA17" s="15"/>
     </row>
     <row r="18" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I18" s="47" t="s">
+      <c r="I18" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="J18" s="19"/>
+      <c r="L18" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="J18" s="48"/>
-      <c r="L18" s="50" t="s">
-        <v>6</v>
-      </c>
-      <c r="M18" s="50"/>
-      <c r="O18" s="28"/>
-      <c r="P18" s="29"/>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="29"/>
-      <c r="T18" s="60" t="s">
-        <v>6</v>
-      </c>
-      <c r="U18" s="60"/>
+      <c r="M18" s="22"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="26"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="26"/>
+      <c r="T18" s="21" t="s">
+        <v>5</v>
+      </c>
+      <c r="U18" s="21"/>
       <c r="V18" s="10"/>
-      <c r="W18" s="48"/>
-      <c r="X18" s="47" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA18" s="54"/>
+      <c r="W18" s="19"/>
+      <c r="X18" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA18" s="15"/>
       <c r="AE18" s="9"/>
     </row>
     <row r="19" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="17">
+      <c r="C19" s="54">
         <v>13</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="I19" s="47"/>
-      <c r="L19" s="26">
+      <c r="D19" s="55"/>
+      <c r="I19" s="18"/>
+      <c r="L19" s="23">
         <v>11</v>
       </c>
-      <c r="M19" s="27"/>
-      <c r="O19" s="28"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="28"/>
-      <c r="R19" s="29"/>
+      <c r="M19" s="24"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="26"/>
       <c r="T19" s="1"/>
       <c r="U19" s="4"/>
       <c r="W19" s="8"/>
-      <c r="X19" s="47"/>
-      <c r="AA19" s="54"/>
+      <c r="X19" s="18"/>
+      <c r="AA19" s="15"/>
       <c r="AE19" s="9"/>
     </row>
     <row r="20" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="19"/>
-      <c r="D20" s="20"/>
-      <c r="I20" s="47"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="29"/>
-      <c r="O20" s="28"/>
-      <c r="P20" s="29"/>
-      <c r="Q20" s="28"/>
-      <c r="R20" s="29"/>
-      <c r="T20" s="26">
+      <c r="C20" s="56"/>
+      <c r="D20" s="57"/>
+      <c r="I20" s="18"/>
+      <c r="L20" s="25"/>
+      <c r="M20" s="26"/>
+      <c r="O20" s="25"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="25"/>
+      <c r="R20" s="26"/>
+      <c r="T20" s="23">
         <v>3</v>
       </c>
-      <c r="U20" s="27"/>
+      <c r="U20" s="24"/>
       <c r="W20" s="8"/>
-      <c r="X20" s="47"/>
-      <c r="AA20" s="54"/>
+      <c r="X20" s="18"/>
+      <c r="AA20" s="15"/>
     </row>
     <row r="21" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="19"/>
-      <c r="D21" s="20"/>
-      <c r="I21" s="47"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="29"/>
-      <c r="O21" s="28"/>
-      <c r="P21" s="29"/>
-      <c r="Q21" s="28"/>
-      <c r="R21" s="29"/>
-      <c r="T21" s="28"/>
-      <c r="U21" s="29"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="57"/>
+      <c r="I21" s="18"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="26"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="26"/>
+      <c r="T21" s="25"/>
+      <c r="U21" s="26"/>
       <c r="W21" s="8"/>
-      <c r="X21" s="47"/>
-      <c r="AA21" s="54"/>
+      <c r="X21" s="18"/>
+      <c r="AA21" s="15"/>
     </row>
     <row r="22" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="19"/>
-      <c r="D22" s="20"/>
-      <c r="I22" s="47"/>
-      <c r="L22" s="28"/>
-      <c r="M22" s="29"/>
-      <c r="O22" s="28"/>
-      <c r="P22" s="29"/>
-      <c r="Q22" s="28"/>
-      <c r="R22" s="29"/>
-      <c r="T22" s="28"/>
-      <c r="U22" s="29"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="57"/>
+      <c r="I22" s="18"/>
+      <c r="L22" s="25"/>
+      <c r="M22" s="26"/>
+      <c r="O22" s="25"/>
+      <c r="P22" s="26"/>
+      <c r="Q22" s="25"/>
+      <c r="R22" s="26"/>
+      <c r="T22" s="25"/>
+      <c r="U22" s="26"/>
       <c r="W22" s="8"/>
-      <c r="X22" s="47"/>
-      <c r="AA22" s="54"/>
+      <c r="X22" s="18"/>
+      <c r="AA22" s="15"/>
     </row>
     <row r="23" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="19"/>
-      <c r="D23" s="20"/>
-      <c r="I23" s="47"/>
-      <c r="L23" s="30"/>
-      <c r="M23" s="31"/>
-      <c r="O23" s="30"/>
-      <c r="P23" s="31"/>
-      <c r="Q23" s="30"/>
-      <c r="R23" s="31"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="57"/>
+      <c r="I23" s="18"/>
+      <c r="L23" s="27"/>
+      <c r="M23" s="28"/>
+      <c r="O23" s="27"/>
+      <c r="P23" s="28"/>
+      <c r="Q23" s="27"/>
+      <c r="R23" s="28"/>
       <c r="T23" s="5"/>
       <c r="U23" s="5"/>
       <c r="W23" s="8"/>
-      <c r="X23" s="47"/>
-      <c r="AA23" s="54"/>
+      <c r="X23" s="18"/>
+      <c r="AA23" s="15"/>
     </row>
     <row r="24" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="19"/>
-      <c r="D24" s="20"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="57"/>
       <c r="E24" t="s">
-        <v>17</v>
-      </c>
-      <c r="F24" s="46" t="s">
-        <v>18</v>
+        <v>13</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>28</v>
       </c>
       <c r="H24" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="47"/>
-      <c r="L24" s="24" t="s">
-        <v>7</v>
-      </c>
-      <c r="M24" s="24"/>
+        <v>11</v>
+      </c>
+      <c r="I24" s="18"/>
+      <c r="L24" s="49" t="s">
+        <v>27</v>
+      </c>
+      <c r="M24" s="49"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
-      <c r="T24" s="50" t="s">
-        <v>7</v>
-      </c>
-      <c r="U24" s="50"/>
+      <c r="T24" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="U24" s="22"/>
       <c r="W24" s="8"/>
-      <c r="X24" s="47"/>
-      <c r="Y24" s="46" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA24" s="54"/>
-      <c r="AB24" s="53"/>
-      <c r="AC24" s="53"/>
+      <c r="X24" s="18"/>
+      <c r="Y24" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA24" s="15"/>
+      <c r="AB24" s="14"/>
+      <c r="AC24" s="14"/>
     </row>
     <row r="25" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="19"/>
-      <c r="D25" s="20"/>
-      <c r="F25" s="46"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="57"/>
+      <c r="F25" s="17"/>
       <c r="H25" s="7"/>
-      <c r="L25" s="26">
+      <c r="L25" s="23">
         <v>12</v>
       </c>
-      <c r="M25" s="27"/>
+      <c r="M25" s="24"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
-      <c r="Q25" s="26">
+      <c r="Q25" s="23">
         <v>7</v>
       </c>
-      <c r="R25" s="27"/>
-      <c r="T25" s="26">
+      <c r="R25" s="24"/>
+      <c r="T25" s="23">
         <v>4</v>
       </c>
-      <c r="U25" s="27"/>
+      <c r="U25" s="24"/>
       <c r="X25" s="11"/>
-      <c r="Y25" s="46"/>
-      <c r="AA25" s="54"/>
+      <c r="Y25" s="17"/>
+      <c r="AA25" s="15"/>
     </row>
     <row r="26" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="19"/>
-      <c r="D26" s="20"/>
-      <c r="F26" s="46"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="57"/>
+      <c r="F26" s="17"/>
       <c r="H26" s="7"/>
-      <c r="L26" s="28"/>
-      <c r="M26" s="29"/>
+      <c r="L26" s="25"/>
+      <c r="M26" s="26"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
-      <c r="Q26" s="28"/>
-      <c r="R26" s="29"/>
-      <c r="T26" s="28"/>
-      <c r="U26" s="29"/>
+      <c r="Q26" s="25"/>
+      <c r="R26" s="26"/>
+      <c r="T26" s="25"/>
+      <c r="U26" s="26"/>
       <c r="X26" s="11"/>
-      <c r="Y26" s="46"/>
-      <c r="AA26" s="54"/>
+      <c r="Y26" s="17"/>
+      <c r="AA26" s="15"/>
     </row>
     <row r="27" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="19"/>
-      <c r="D27" s="20"/>
-      <c r="F27" s="46"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="57"/>
+      <c r="F27" s="17"/>
       <c r="H27" s="7"/>
-      <c r="L27" s="28"/>
-      <c r="M27" s="29"/>
-      <c r="Q27" s="28"/>
-      <c r="R27" s="29"/>
-      <c r="T27" s="28"/>
-      <c r="U27" s="29"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="26"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="26"/>
+      <c r="T27" s="25"/>
+      <c r="U27" s="26"/>
       <c r="X27" s="11"/>
-      <c r="Y27" s="46"/>
-      <c r="AA27" s="54"/>
+      <c r="Y27" s="17"/>
+      <c r="AA27" s="15"/>
     </row>
     <row r="28" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="19"/>
-      <c r="D28" s="20"/>
-      <c r="F28" s="46"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="57"/>
+      <c r="F28" s="17"/>
       <c r="H28" s="7"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="29"/>
-      <c r="Q28" s="28"/>
-      <c r="R28" s="29"/>
-      <c r="T28" s="28"/>
-      <c r="U28" s="29"/>
+      <c r="L28" s="25"/>
+      <c r="M28" s="26"/>
+      <c r="Q28" s="25"/>
+      <c r="R28" s="26"/>
+      <c r="T28" s="25"/>
+      <c r="U28" s="26"/>
       <c r="X28" s="11"/>
-      <c r="Y28" s="46"/>
-      <c r="AA28" s="54"/>
+      <c r="Y28" s="17"/>
+      <c r="AA28" s="15"/>
     </row>
     <row r="29" spans="3:31" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="21"/>
-      <c r="D29" s="22"/>
-      <c r="F29" s="46"/>
+      <c r="C29" s="58"/>
+      <c r="D29" s="59"/>
+      <c r="F29" s="17"/>
       <c r="H29" s="7"/>
-      <c r="L29" s="30"/>
-      <c r="M29" s="31"/>
-      <c r="Q29" s="30"/>
-      <c r="R29" s="31"/>
-      <c r="T29" s="30"/>
-      <c r="U29" s="31"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="28"/>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="28"/>
+      <c r="T29" s="27"/>
+      <c r="U29" s="28"/>
       <c r="X29" s="11"/>
-      <c r="Y29" s="46"/>
-      <c r="AA29" s="54"/>
+      <c r="Y29" s="17"/>
+      <c r="AA29" s="15"/>
     </row>
     <row r="30" spans="3:31" x14ac:dyDescent="0.3">
-      <c r="F30" s="46"/>
+      <c r="F30" s="17"/>
       <c r="H30" s="7"/>
-      <c r="L30" s="25">
-        <v>3100</v>
-      </c>
-      <c r="M30" s="25"/>
-      <c r="N30" s="25"/>
-      <c r="O30" s="25"/>
-      <c r="P30" s="25"/>
-      <c r="Q30" s="25"/>
-      <c r="R30" s="25"/>
-      <c r="S30" s="25"/>
-      <c r="T30" s="25"/>
-      <c r="U30" s="25"/>
+      <c r="L30" s="50">
+        <v>3070</v>
+      </c>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="50"/>
+      <c r="Q30" s="50"/>
+      <c r="R30" s="50"/>
+      <c r="S30" s="50"/>
+      <c r="T30" s="50"/>
+      <c r="U30" s="50"/>
       <c r="X30" s="11"/>
-      <c r="Y30" s="46"/>
-      <c r="AA30" s="54"/>
+      <c r="Y30" s="17"/>
+      <c r="AA30" s="15"/>
     </row>
     <row r="31" spans="3:31" x14ac:dyDescent="0.3">
-      <c r="C31" s="61" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="61"/>
-      <c r="E31" s="61"/>
-      <c r="F31" s="61"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="61"/>
-      <c r="J31" s="61"/>
-      <c r="L31" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="M31" s="16"/>
-      <c r="O31" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
+      <c r="C31" s="60" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="60"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="L31" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="M31" s="53"/>
+      <c r="O31" s="52" t="s">
+        <v>16</v>
+      </c>
+      <c r="P31" s="52"/>
+      <c r="Q31" s="52"/>
+      <c r="R31" s="52"/>
       <c r="S31" s="3"/>
-      <c r="T31" s="23" t="s">
-        <v>19</v>
-      </c>
-      <c r="U31" s="23"/>
-      <c r="AA31" s="54"/>
+      <c r="T31" s="48" t="s">
+        <v>14</v>
+      </c>
+      <c r="U31" s="48"/>
+      <c r="AA31" s="15"/>
     </row>
     <row r="32" spans="3:31" x14ac:dyDescent="0.3">
       <c r="C32" t="s">
-        <v>28</v>
-      </c>
-      <c r="F32" s="51" t="s">
+        <v>22</v>
+      </c>
+      <c r="F32" s="61" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="61"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="61"/>
+      <c r="J32" s="61"/>
+      <c r="L32" t="s">
+        <v>18</v>
+      </c>
+      <c r="M32" t="s">
+        <v>8</v>
+      </c>
+      <c r="O32" t="s">
+        <v>8</v>
+      </c>
+      <c r="R32" t="s">
+        <v>15</v>
+      </c>
+      <c r="T32" t="s">
+        <v>15</v>
+      </c>
+      <c r="U32" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA32" s="15"/>
+    </row>
+    <row r="33" spans="15:27" x14ac:dyDescent="0.3">
+      <c r="O33" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="P33" s="51"/>
+      <c r="Q33" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="G32" s="51"/>
-      <c r="H32" s="51"/>
-      <c r="I32" s="51"/>
-      <c r="J32" s="51"/>
-      <c r="L32" t="s">
-        <v>23</v>
-      </c>
-      <c r="M32" t="s">
-        <v>10</v>
-      </c>
-      <c r="O32" t="s">
-        <v>10</v>
-      </c>
-      <c r="R32" t="s">
-        <v>20</v>
-      </c>
-      <c r="T32" t="s">
-        <v>20</v>
-      </c>
-      <c r="U32" t="s">
-        <v>9</v>
-      </c>
-      <c r="AA32" s="54"/>
-    </row>
-    <row r="33" spans="15:27" x14ac:dyDescent="0.3">
-      <c r="O33" s="14" t="s">
-        <v>12</v>
-      </c>
-      <c r="P33" s="14"/>
-      <c r="Q33" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="R33" s="14"/>
-      <c r="AA33" s="54"/>
+      <c r="R33" s="51"/>
+      <c r="AA33" s="15"/>
     </row>
     <row r="34" spans="15:27" x14ac:dyDescent="0.3">
       <c r="O34" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P34" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="Q34" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="R34" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA34" s="54"/>
+        <v>6</v>
+      </c>
+      <c r="AA34" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="C19:D29"/>
+    <mergeCell ref="C31:J31"/>
+    <mergeCell ref="F32:J32"/>
+    <mergeCell ref="AE11:AE12"/>
+    <mergeCell ref="L5:U6"/>
+    <mergeCell ref="M7:T9"/>
+    <mergeCell ref="O14:P23"/>
+    <mergeCell ref="T31:U31"/>
+    <mergeCell ref="L24:M24"/>
+    <mergeCell ref="T24:U24"/>
+    <mergeCell ref="L30:U30"/>
+    <mergeCell ref="T20:U22"/>
+    <mergeCell ref="T25:U29"/>
+    <mergeCell ref="Q25:R29"/>
+    <mergeCell ref="L19:M23"/>
+    <mergeCell ref="L25:M29"/>
+    <mergeCell ref="O31:R31"/>
+    <mergeCell ref="L31:M31"/>
+    <mergeCell ref="AD5:AD6"/>
+    <mergeCell ref="AD7:AD8"/>
+    <mergeCell ref="AD9:AD10"/>
+    <mergeCell ref="L14:M16"/>
+    <mergeCell ref="AD11:AD12"/>
     <mergeCell ref="AA5:AA34"/>
     <mergeCell ref="C2:Y2"/>
     <mergeCell ref="Y24:Y30"/>
@@ -1635,31 +1658,8 @@
     <mergeCell ref="Q14:R23"/>
     <mergeCell ref="T13:U17"/>
     <mergeCell ref="X18:X24"/>
-    <mergeCell ref="AD5:AD6"/>
-    <mergeCell ref="AD7:AD8"/>
-    <mergeCell ref="AD9:AD10"/>
-    <mergeCell ref="L14:M16"/>
-    <mergeCell ref="AD11:AD12"/>
-    <mergeCell ref="AE11:AE12"/>
-    <mergeCell ref="L5:U6"/>
-    <mergeCell ref="M7:T9"/>
-    <mergeCell ref="O14:P23"/>
-    <mergeCell ref="T31:U31"/>
-    <mergeCell ref="L24:M24"/>
-    <mergeCell ref="T24:U24"/>
-    <mergeCell ref="L30:U30"/>
-    <mergeCell ref="T20:U22"/>
-    <mergeCell ref="T25:U29"/>
-    <mergeCell ref="Q25:R29"/>
-    <mergeCell ref="L19:M23"/>
-    <mergeCell ref="L25:M29"/>
     <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="O31:R31"/>
-    <mergeCell ref="L31:M31"/>
     <mergeCell ref="O33:P33"/>
-    <mergeCell ref="C19:D29"/>
-    <mergeCell ref="C31:J31"/>
-    <mergeCell ref="F32:J32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>